<commit_message>
fix(input data)Changed student_name to student_number
</commit_message>
<xml_diff>
--- a/static/files/template_student_data.xlsx
+++ b/static/files/template_student_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E28083-2A78-4AAD-8B5D-0E93A43D2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FCC7A9-F826-4C12-A25E-71C2D99FC085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>student_name</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>adjectives</t>
+  </si>
+  <si>
+    <t>student_number</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,28 +450,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "fix(input data)Changed student_name to student_number"
This reverts commit 8a888a1c8d8e896738ed5e4aa0564d553decba88.
</commit_message>
<xml_diff>
--- a/static/files/template_student_data.xlsx
+++ b/static/files/template_student_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks.r\Documents\REPORT_WRITING_APPLICATION\Batch_Report\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FCC7A9-F826-4C12-A25E-71C2D99FC085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E28083-2A78-4AAD-8B5D-0E93A43D2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA61B80E-0392-4D06-90DD-9D43CDF00CCC}"/>
   </bookViews>
@@ -38,6 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>student_name</t>
+  </si>
+  <si>
     <t>year</t>
   </si>
   <si>
@@ -57,9 +60,6 @@
   </si>
   <si>
     <t>adjectives</t>
-  </si>
-  <si>
-    <t>student_number</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,28 +450,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>